<commit_message>
fixed problem with empty models and marks but existent image
</commit_message>
<xml_diff>
--- a/Agco.xlsx
+++ b/Agco.xlsx
@@ -1016,9 +1016,17 @@
           <t>V581705490</t>
         </is>
       </c>
-      <c r="B32" s="11" t="n"/>
-      <c r="C32" s="11" t="n"/>
-      <c r="D32" s="11" t="n"/>
+      <c r="B32" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson, Valtra</t>
+        </is>
+      </c>
+      <c r="C32" s="11" t="inlineStr">
+        <is>
+          <t>8370P, 8400P, 9390R, Rogator 635 (MY19), RG 635, 6465 Dyna-6, 6475 Dyna-6, MF 6480 T3 Agco Power, MF 6497 T2 Agco Power, MF 6490 T2 Agco Power, MF 6495 T2 Agco Power, MF 6485 T2 Agco Power, 6485, MF 6490 T3 Agco Power, MF 6495 T3 Agco Power, MF 6470 T3 Agco Power, MF 6460 T3 Agco Power, MF 7465 T3 SISU, MF 7475 T3 SISU, MF 7480 T3 SISU, MF 7485 T3, MF 7490 T3, MF 7495 T3, MF 7497, MF 7499, MF 9695, MF 9795, MF 5465 Dyna-4, MF 5475 Dyna-4, MF 5460 T3 SISU, 5475, 5470, MF 5470 T3, MF 5480 T3, MF 5470 SISU, MF 7265 (2009-2011), MF 7345 S MCS (2011-2014), MF 7347 S MCS (2012-2014), MF 7360 T4I (2012), MF 7360 PL T4I (2012), MF 7370 T4I (2012), MF 7345 S (2011-2014), MF 7347 S (2012-2014), MF 7360 T4I (2013-2014), MF 7360 PL T4I (2013-2014), MF 7370 T4I (2013-2014), MF 7360 PLI T4I (2013-2014), MF 7345 S (09/14 - 08/17), MF 7345 S MCS (09/14 - 08/17), MF 7347 S (09/14 - 08/17), MF 7347 S MCS (09/14 - 08/17), MF 7360 T4F (2015-2017), MF 7360 PL T4F (2015-2017), MF 7360 PLI T4F (2015-2017), MF 7370 T4F (2015-2017), MF 7370 PL (09/14 - 08/17), MF 7344 TF4 (2018-2021), MF 7345 S T4F (2018-2021), MF 7347 S T4F (2018-2021), MF 7360 T4F (2018-2021), MF 7360 PL/PLI T4F (2018-2021), MF 7370 T4F (2018-2021), MF 7370 ST5 (2021-9999), MF 7344 (09/15 - 08/17), MF 7247 S (2008-2011), MF 7274, MF 7260 (2005-2011), MF 7270 (2005-2011), MF 7370 PLI (2017), MF 7280 (09/08 - 03/13), MF 7282 (09/08 - 03/13), MF 7278, MF Activa S 7345 MCS, MF Activa S 7347 MCS, MF Beta 7370 PL, MF Beta 7370 PLI, M120, M120E, M120H, M130, M150, T120, T130, T140E, T150, T160, T170, T180, T190, T120C, T120CH, T130C, T130CH, T140EC, T140ECH, T160C, T160CH, T170C, T170CH, T150C, T150CH, XM130, XM150, T131C, T161C, T171C, T121H, T131H, T151EH, T161H, T171H, T191H, T121C, T161LS, T171LS, T191LS, T132V, T152V, T162EV, T172V, T182V, T202V, T132D, T152D, T162D, T172D, T182D, T202D, T193H, T213V, T183D, T203D</t>
+        </is>
+      </c>
+      <c r="D32" s="11" t="inlineStr"/>
     </row>
     <row r="33" ht="18.75" customHeight="1">
       <c r="A33" s="3" t="inlineStr">
@@ -1026,9 +1034,13 @@
           <t>17C-636</t>
         </is>
       </c>
-      <c r="B33" s="11" t="n"/>
-      <c r="C33" s="11" t="n"/>
-      <c r="D33" s="11" t="n"/>
+      <c r="B33" s="11" t="inlineStr"/>
+      <c r="C33" s="11" t="inlineStr"/>
+      <c r="D33" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="18.75" customHeight="1">
       <c r="A34" s="3" t="inlineStr">
@@ -1036,17 +1048,25 @@
           <t>17C000636B</t>
         </is>
       </c>
-      <c r="B34" s="11" t="n"/>
-      <c r="C34" s="11" t="n"/>
-      <c r="D34" s="11" t="n"/>
+      <c r="B34" s="11" t="inlineStr"/>
+      <c r="C34" s="11" t="inlineStr"/>
+      <c r="D34" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="18.75" customHeight="1">
       <c r="A35" s="4" t="n">
         <v>86564938</v>
       </c>
-      <c r="B35" s="11" t="n"/>
-      <c r="C35" s="11" t="n"/>
-      <c r="D35" s="11" t="n"/>
+      <c r="B35" s="11" t="inlineStr"/>
+      <c r="C35" s="11" t="inlineStr"/>
+      <c r="D35" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="18.75" customHeight="1">
       <c r="A36" s="3" t="inlineStr">
@@ -1054,25 +1074,57 @@
           <t>40502PF</t>
         </is>
       </c>
-      <c r="B36" s="11" t="n"/>
-      <c r="C36" s="11" t="n"/>
-      <c r="D36" s="11" t="n"/>
+      <c r="B36" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C36" s="11" t="inlineStr">
+        <is>
+          <t>9300R, MF 35, TE20, MF 135, MF 165, MF 175, MF 178, MF 155, MF 175S, MF 148, MF 168, MF 188, MF 152, MF 158, MF 185, MF 165 MK3, MF 168 4WD, MF 168F, MF 145 MK3/V, MF 158V, MF 254S 4WD, MF 294 4WD, MF 264, MF 264 4WD, MF 550, MF 575, MF 560, MF 575 4WD, MF 590 4WD, MF 595, MF 595 4WD, MF 565, MF 592, MF 592 4WD, MF 698, MF 698 4WD, MF 698T, MF 698T 4WD, MF 699, MF 699 4WD, MF 670 4WD, MF 690, MF 2620/2625, MF 2640/2645 2WD, MF 2640/2645 4WD, MF 2620/2625 4WD, MF 2680 2WD, MF 2680 4WD, MF 2720/2725, MF 354F 2WD, MF 354F 4WD, MF 364F 2WD, MF 364F 4WD, MF 354S 2WD, MF 354S 4WD, MF 364S 2WD, MF 364S 4WD, MF 394S 2WD, MF 364V 2WD, MF 364V 4WD, MF 3080 2WD, MF 3080 4WD, MF 3090 2WD, MF 3090 4WD, MF 3610 2WD, MF 3610 4WD, MF 3630 2WD, MF 3630 4WD, MF 3650 2WD, MF 3650 4WD, MF 3680 2WD, MF 3680 4WD, MF 1200, MF 1250, MF 333 2WD, MF 353 2WD, MF 353 4WD, MF 363 2WD, MF 363 4WD, MF 353S 2WD, MF 353S 4WD, MF 1114 2WD, MF 1114 4WD, MF 1134 2WD, MF 1134 4WD, MF 1014 2WD, MF 1014 4WD, MF 4315 2WD, MF 4315 4WD, MF 4325 2WD, MF 4325 4WD, MF 4335 2WD, MF 4335 4WD, MF 4345 2WD, MF 4345 4WD, MF 4355 2WD, MF 4355 4WD, MF 4360 2WD, MF 4360 4WD, MF 4365 2WD, MF 4365 4WD, MF 4370 2WD, MF 4370 4WD, MF 4215 2WD, MF 4215 4WD, MF 4220 2WD, MF 4220 4WD, MF 4225 2WD, MF 4225 4WD, MF 4235 2WD, MF 4235 4WD, MF 4240 2WD, MF 4240 4WD, MF 4245 2WD, MF 4245 4WD, MF 4255 2WD, MF 4255 4WD, MF 4260 2WD, MF 4260 4WD, MF 4265 2WD, MF 4265 4WD, MF 4270 2WD, MF 4270 4WD, MF 8250 4WD, MF 9690, MF 9790, MF 9895, MF 9695, MF 9795, MF 2210, MF 1035, MF 1045, MF 245, MF 265, MF 285, MF 235, MF 255, MF 260, MF 275 4WD, MF 275 2WD, MF 298 2WD, MF 298 4WD, MF 290 2WD, MF 298, MF 290 4WD, MF 250, MF 230, MF 270, MF 350 2WD, MF 350 4WD, MF 375 2WD, MF 375 4WD, MF 390 2WD, MF 390 4WD, MF 398 2WD, MF 398 4WD, MF 399 2WD, MF 399 4WD, MF 360 2WD, MF 360 4WD, MF 365 2WD, MF 365 4WD, MF 355 2WD, MF 355 4WD, MF 390T 2WD, MF 390T 4WD, MF 362 2WD, MF 362 4WD, MF 340 4WD, MF 340 2WD, MF 372 N 2WD, MF 372 N 4WD, MF 382 N 4WD, MF 362 N 2WD, MF 362 N 4WD, MF 342 2WD, MF 352 2WD</t>
+        </is>
+      </c>
+      <c r="D36" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="18.75" customHeight="1">
       <c r="A37" s="4" t="n">
         <v>7702160</v>
       </c>
-      <c r="B37" s="11" t="n"/>
-      <c r="C37" s="11" t="n"/>
-      <c r="D37" s="11" t="n"/>
+      <c r="B37" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C37" s="11" t="inlineStr">
+        <is>
+          <t>Favorit 920 Vario, Favorit 924 Vario, Favorit 926 Vario, MF 2640/2645 2WD, MF 394S 2WD, MF 3630 2WD, MF 3650 2WD, MF 3680 2WD, MF 3645 2WD, MF 3655 2WD, MF 3670 2WD, MF 3690 2WD, MF 8120 2WD, MF 8140 2WD, MF 8150 2WD, MF 8160 2WD, MF 4325 2WD, MF 4325 4WD, MF 4335 2WD, MF 4335 4WD, MF 4345 2WD, MF 4345 4WD, MF 4355 2WD, MF 4355 4WD, MF 4360 2WD, MF 4360 4WD, MF 4370 2WD, MF 4370 4WD, MF 4225 2WD, MF 4235 2WD, MF 4240 2WD, MF 4245 2WD, MF 4255 2WD, MF 4260 2WD, MF 4265 2WD, MF 4270 2WD, MF 8250 2WD, MF 8250 4WD, MF 8280 4WD, MF 8270 4WD, MF 8260 2WD, MF 8240 2WD, MF 8240 4WD, MF 8220 2WD, MF 8220 4WD, MF 8210 2WD, MF 8210 4WD, MF 9690, MF 185 SII, MF 375 2WD, MF 390 2WD, MF 398 2WD, MF 399 2WD, MF 360 2WD, MF 365 2WD, MF 390T 2WD, MF 362 2WD</t>
+        </is>
+      </c>
+      <c r="D37" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="18.75" customHeight="1">
       <c r="A38" s="4" t="n">
         <v>70921210</v>
       </c>
-      <c r="B38" s="11" t="n"/>
-      <c r="C38" s="11" t="n"/>
-      <c r="D38" s="11" t="n"/>
+      <c r="B38" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C38" s="11" t="inlineStr">
+        <is>
+          <t>PLNTR MOMENTUM 16-30 FT 40', PLNTR MOMENTUM 16-70 FT 40', PLNTR MOMENTUM 16-76 FT 40', PLNTR MOMENTUM 24-20 FT 40', PLNTR MOMENTUM 24-22 FT 40', PLNTR MOMENTUM 32-15 FT 40', PLNTR MOMENTUM 24-30 FT 60', PLNTR MOMENTUM 24-70 FT 60', PLNTR MOMENTUM 24-76 FT 60', PLNTR MOMENTUM 36-20 FT 60', PLNTR MOMENTUM 36-22 FT 60', PLNTR MOMENTUM 48-15 FT 60', 8370P, 8400P, 9300R, 9390R, 9470X, 990 (Serial No. JHBxxx001 to JBHxxx999), 1270 (Serial No. JHBxxx001 to JBHxxx999), 1290 XD (Serial No. JHBxxx001 to JBHxxx999), 12130 (Serial No. JHBxxx001 to JBHxxx999), 1290, Squadra 1290 UD, MF 35, TE20, MF 135, MF 165, MF 175, MF 145, MF 178, MF 155, MF 175S, MF 148, MF 168, MF 188, MF 152, MF 158, MF 185, MF 165 MK3, MF 168 4WD, MF 168F, MF 145 MK3/V, MF 158V, MF 154S 2WD, MF 154S 4WD, MF 174S 2WD, MF 185 4WD, MF 184S 2WD, MF 185S 4WD, MF 174S, MF 154F, MF 174F, MF 184F, MF 194F, MF 194S, MF 164F, MF 164F 4WD, MF 234S, MF 254S 4WD, MF 294 4WD, MF 264, MF 264 4WD, MF 264S 2WD, MF 264S 4WD, MF 550, MF 575, MF 590, MF 560, MF 575 4WD, MF 590 4WD, MF 595, MF 595 4WD, MF 565, MF 592, MF 592 4WD, MF 698, MF 698 4WD, MF 698T, MF 698T 4WD, MF 699, MF 699 4WD, MF 670 4WD, MF 690, MF 2620/2625, MF 2640/2645 2WD, MF 2640/2645 4WD, MF 2620/2625 4WD, MF 2680 2WD, MF 2680 4WD, MF 2720/2725, MF 354F 2WD, MF 354F 4WD, MF 364F 2WD, MF 364F 4WD, MF 374F 2WD, MF 374F 4WD, MF 384F 2WD, MF 384F 4WD, MF 394F 2WD, MF 394F 4WD, MF 354S 2WD, MF 354S 4WD, MF 364S 2WD, MF 364S 4WD, MF 374S 2WD, MF 374S 4WD, MF 384S 2WD, MF 384S 4WD, MF 394S 2WD, MF 394S 4WD, MF 354V 2WD, MF 354V 4WD, MF 364V 2WD, MF 364V 4WD, MF 374V 2WD, MF 374V 4WD, MF 3610 2WD, MF 3610 4WD, MF 3630 2WD, MF 3630 4WD, MF 3650 2WD, MF 3650 4WD, MF 3680 2WD, MF 3680 4WD, MF 3645 2WD, MF 3645 4WD, MF 3655 2WD, MF 3655 4WD, MF 3670 2WD, MF 3670 4WD, MF 3690 2WD, MF 3690 4WD, MF 3635 2WD, MF 3635 4WD, MF 1200, MF 1250, MF 194 2WD, MF 194 4WD, MF 294 2WD, MF 284S 2WD, MF 284S 4WD, MF 263, MF 263 4WD, MF 333 2WD, MF 353 2WD, MF 353 4WD, MF 363 2WD, MF 363 4WD, MF 373 2WD, MF 373 4WD, MF 383 2WD, MF 383 4WD, MF 393 2WD, MF 393 4WD, MF 353S 2WD, MF 353S 4WD, MF 363S 4WD, MF 373S 2WD, MF 373S 4WD, MF 377 2WD, MF 377 4WD, MF 387 2WD, MF 387 4WD, MF 397 2WD, MF 397 4WD, MF 8170 4WD, MF 8110 2WD, MF 8110 4WD, MF 8120 2WD, MF 8120 4WD, MF 8130 2WD, MF 8130 4WD, MF 8140 2WD, MF 8140 4WD, MF 8150 2WD, MF 8150 4WD, MF 8160 2WD, MF 8160 4WD, MF 4315 2WD, MF 4315 4WD, MF 4325 2WD, MF 4325 4WD, MF 4335 2WD, MF 4335 4WD, MF 4345 2WD, MF 4345 4WD, MF 4355 2WD, MF 4355 4WD, MF 4360 2WD, MF 4360 4WD, MF 4365 2WD, MF 4365 4WD, MF 4370 2WD, MF 4370 4WD, MF 4215 2WD, MF 4215 4WD, MF 4220 2WD, MF 4220 4WD, MF 4225 2WD, MF 4225 4WD, MF 4235 2WD, MF 4235 4WD, MF 4240 2WD, MF 4240 4WD, MF 4245 2WD, MF 4245 4WD, MF 4255 2WD, MF 4255 4WD, MF 4260 2WD, MF 4260 4WD, MF 4265 2WD, MF 4265 4WD, MF 4270 2WD, MF 4270 4WD, MF 6290 2WD, MF 6290 4WD, MF 6280 2WD, MF 6280 4WD, MF 6270 2WD, MF 6270 4WD, MF 6265 2WD, MF 6265 4WD, MF 6260 2WD, MF 6260 4WD, MF 6255 2WD, MF 6255 4WD, MF 6245 2WD, MF 6245 4WD, MF 6235 2WD, MF 6235 4WD, MF 8260 4WD, MF 8250 2WD, MF 8250 4WD, MF 8280 4WD, MF 8270 4WD, MF 8260 2WD, MF 8240 2WD, MF 8240 4WD, MF 8220 2WD, MF 8220 4WD, MF 8210 2WD, MF 8210 4WD, MF 6465 T2 Perkins, MF 6475 T2 Perkins, MF 6480 T2 Perkins, MF 9540, MF 9560, MF 9690, MF 9790, MF 9895, MF 9695, MF 9795, MF 5709 S Dyna-4, MF 5709 S Dyna-6, MF 6612 Dyna-4, MF 6613 Dyna-6, MF 6613 Dyna-4, MF 6614 Dyna-VT, MF 6614 Dyna-6, MF 6615 Dyna-4, MF 6615 Dyna-VT, MF 6615 Dyna-6, MF 6616 Dyna-VT, MF 6616 Dyna-6, MF 5709 SL Dyna-4, MF 5710 SL Dyna-4, MF 5710 SL Dyna-6, MF 5711 SL Dyna-4, MF 5711 SL Dyna-6, MF 5712 SL Dyna-4, MF 5712 SL Dyna-6, MF 5713 SL Dyna-4, MF 5713 SL Dyna-6, MF 6712 S Dyna-4, MF 6713 S Dyna-4, MF 6714 S Dyna-4 T4F, MF 6715 S Dyna-4 T4F, MF 6713 S Dyna-6, MF 6713 S Dyna-VT, MF 6714 S Dyna-6, MF 6714 S Dyna-VT, MF 6715 S Dyna-6 T4F, MF 6715 S Dyna-VT, MF 6716 S Dyna-6 T4F, MF 6716 S Dyna-VT T4F, MF 6718 S Dyna-6, MF 6718 S Dyna-VT, MF 6714 S Dyna-6 T4F, MF 6714 S Dyna-VT T4F, MF 7719 Dyna-6, MF 7715 DYNA-4, MF 7716 Dyna-6, MF 7714 Dyna-4, MF 7715 Dyna-4, MF 7726 Dyna-VT, MF6713 S Dyna-6 T5, MF 6713 S Dyna-VT T5, MF 6714 S Dyna-6 T5, MF 6714 S Dyna-VT T5, MF 6715 S Dyna-6 T5, MF 6715 S Dyna-VT T5, MF 6716 S Dyna-6 T5, MF 6716 S Dyna-VT T5, MF 6718 S Dyna-6 T5, MF 6718 S Dyna-VT T5, MF 7714 S Dyna-4, MF 7719 S Dyna-VT T5, MF 7714 S Dyna-4 T5, MF 7715 S Dyna-VT T5, MF 7715 S Dyna-6 T5, MF 7716 S Dyna-VT T5, MF 7716 S Dyna-6 T5, MF 7718 S Dyna-VT T5, MF 7718 S Dyna-6 T5, MF 5450 T3, MF 2170XD, MF 2150 CE, MF 2160 CE, MF 2170CE, MF 185 SII, MF 190CE, MF 186CE, MF 187CE, MF 2140 CE, MF1547, MF 245, MF 265, MF 285, MF 235, MF 255, MF 260, MF 275 4WD, MF 275 2WD, MF 298 2WD, MF 298 4WD, MF 290 2WD, MF 298, MF 290 4WD, MF 250, MF 230, MF 270, MF8727, MF 350 2WD, MF 350 4WD, MF 375 2WD, MF 375 4WD, MF 390 2WD, MF 390 4WD, MF 398 2WD, MF 398 4WD, MF 399 2WD, MF 399 4WD, MF 360 2WD, MF 360 4WD, MF 365 2WD, MF 365 4WD, MF 355 2WD, MF 355 4WD, MF 390T 2WD, MF 390T 4WD, MF 362 2WD, MF 362 4WD, MF 340 4WD, MF 340 2WD, MF 372 N 2WD, MF 372 N 4WD, MF 382 N 4WD, MF 362 N 2WD, MF 362 N 4WD, MF 342 2WD, MF 352 2WD, MF 7274, MF 7280 (09/08 - 03/13), MF 7282 (09/08 - 03/13), MF 7278, MF 7272</t>
+        </is>
+      </c>
+      <c r="D38" s="11" t="inlineStr"/>
     </row>
     <row r="39" ht="18.75" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
@@ -1080,9 +1132,9 @@
           <t>SN1678</t>
         </is>
       </c>
-      <c r="B39" s="11" t="n"/>
-      <c r="C39" s="11" t="n"/>
-      <c r="D39" s="11" t="n"/>
+      <c r="B39" s="11" t="inlineStr"/>
+      <c r="C39" s="11" t="inlineStr"/>
+      <c r="D39" s="11" t="inlineStr"/>
     </row>
     <row r="40" ht="18.75" customHeight="1">
       <c r="A40" s="3" t="inlineStr">
@@ -1090,9 +1142,21 @@
           <t>SN6306</t>
         </is>
       </c>
-      <c r="B40" s="11" t="n"/>
-      <c r="C40" s="11" t="n"/>
-      <c r="D40" s="11" t="n"/>
+      <c r="B40" s="11" t="inlineStr">
+        <is>
+          <t>Challenger, Gleaner, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C40" s="11" t="inlineStr">
+        <is>
+          <t>LB34BXD, 2270XD, 4200 Pickup Header, MF 9435, MF 3000, MF 4200S-13 Pick Up Header, MF 2170XD, MF 2290, MF 2150</t>
+        </is>
+      </c>
+      <c r="D40" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="41" ht="18.75" customHeight="1">
       <c r="A41" s="3" t="inlineStr">
@@ -1100,17 +1164,33 @@
           <t>40587PF</t>
         </is>
       </c>
-      <c r="B41" s="11" t="n"/>
-      <c r="C41" s="11" t="n"/>
-      <c r="D41" s="11" t="n"/>
+      <c r="B41" s="11" t="inlineStr">
+        <is>
+          <t>Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C41" s="11" t="inlineStr">
+        <is>
+          <t>MF 135, MF 152, MF 158, MF 168 4WD, MF 168F, MF 145 MK3/V, MF 158V, MF 560, MF 595, MF 595 4WD, MF 592, MF 592 4WD, MF 698, MF 698 4WD, MF 698T, MF 698T 4WD, MF 699, MF 699 4WD, MF 8250 2WD, MF 8250 4WD, MF 8240 2WD, MF 8240 4WD, MF 8220 2WD, MF 8220 4WD, MF 8210 2WD, MF 8210 4WD, MF 6497 T2 Agco Power, MF 6499 T2 Agco Power, MF 6490 T2 Agco Power, MF 6495 T2 Agco Power, MF 6485 T2 Agco Power, MF 245, MF 235, MF 255, MF 260, MF 290 2WD, MF 290 4WD, MF 250</t>
+        </is>
+      </c>
+      <c r="D41" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="42" ht="18.75" customHeight="1">
       <c r="A42" s="4" t="n">
         <v>702035</v>
       </c>
-      <c r="B42" s="11" t="n"/>
-      <c r="C42" s="11" t="n"/>
-      <c r="D42" s="11" t="n"/>
+      <c r="B42" s="11" t="inlineStr"/>
+      <c r="C42" s="11" t="inlineStr"/>
+      <c r="D42" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="43" ht="18.75" customHeight="1">
       <c r="A43" s="3" t="inlineStr">
@@ -1118,9 +1198,17 @@
           <t>393761X1</t>
         </is>
       </c>
-      <c r="B43" s="11" t="n"/>
-      <c r="C43" s="11" t="n"/>
-      <c r="D43" s="11" t="n"/>
+      <c r="B43" s="11" t="inlineStr">
+        <is>
+          <t>Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C43" s="11" t="inlineStr">
+        <is>
+          <t>MF 698, MF 698 4WD, MF 690, MF 3425, MF 3435, MF 3445, MF 3455, MF 3435C, MF 3445C, MF 3455C, MF 3425C, MF 6110 2WD, MF 6110 4WD, MF 6120 2WD, MF 6120 4WD, MF 6130 2WD, MF 6130 4WD, MF 6140 2WD, MF 6140 4WD, MF 6150 2WD, MF 6150 4WD, MF 6160 2WD, MF 6160 4WD, MF 6170 2WD, MF 6170 4WD, MF 6180 2WD, MF 6180 4WD, MF 6190 2WD, MF 6190 4WD, MF 9540, MF 9560, MF 9690</t>
+        </is>
+      </c>
+      <c r="D43" s="11" t="inlineStr"/>
     </row>
     <row r="44" ht="18.75" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
@@ -1128,9 +1216,17 @@
           <t>339139X1</t>
         </is>
       </c>
-      <c r="B44" s="11" t="n"/>
-      <c r="C44" s="11" t="n"/>
-      <c r="D44" s="11" t="n"/>
+      <c r="B44" s="11" t="inlineStr">
+        <is>
+          <t>Challenger, Fendt, Gleaner, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C44" s="11" t="inlineStr">
+        <is>
+          <t>RG700, RG700B, MT455D, MT465D, MT445B, MT455B, MT465B, MT445B-T3, MT455B-T3 Dyna-4, MT465B-T3 Dyna-4, MT555D Dyna-6, MT565D Dyna-6, MT575D Dyna-6, MT585D Dyna-6, MT555D CVT, MT565D CVT, MT575D CVT, MT585D CVT, MT515D Dyna-4, MT525D Dyna-4, MT525D Dyna-6, MT535D Dyna-6, MT545D Dyna-6, MT525D Dyna-VT, MT535D Dyna-VT, MT545D Dyna-VT, MT575E Dyna-6, MT525E Dyna-4, MT525E Dyna-6, MT545E Dyna-6, MT545B Dyna-6, MT525B Dyna-6, MT525B Dyna-CVT, MT545B Dyna-CVT, MT555B Dyna-CVT T3 CAT, MT565B Dyna-CVT T3 CAT, MT575B Dyna-CVT T3 CAT, MT555B Dyna-6 T3 CAT, MT565B Dyna-6 T3 CAT, MT575B Dyna-6 T3 CAT, MT525B Dyna-6 T3 CAT, MT545B Dyna-6 T3 CAT, MT525B Dyna-CVT T3 CAT, MT545B Dyna-CVT T3 CAT, MT595B Dyna-6 T3 SISU, MT595B Dyna-CVT T3 SISU , MT645D T4I, MT655D T4I, MT665D T4I / T2, MT675D T4I, MT685D T4I / T2, MT665E, MT645C, MT655C T3 CVT, MT665C T3 / T2 CVT, MT675C T3 CVT, MT645E, MT665E T4F CVT, PTD12 Roller, IDEAL 7, IDEAL 8, IDEAL 9, S96, S97, S98, A66, A76, 5100 Draper Header, 3308 Corn Header, 3312 Corn Header, 3308C Corn Header, 3312C Corn Header, MF 2650, MF 2660, MF 6712 ECO4, MF 7465 T3 SISU, MF 7475 T3 SISU, MF 7480 T3 SISU, MF 7485 T3, MF 7490 T3, MF 7495 T3, MF 7465 T3, MF 7475 T3, MF 7480 T3, MF 7499, MF 5710 ECO3, MF 5710 ECO4, MF 5711 ECO4, MF 5609 Dyna-4, MF 5610 Dyna-4, MF 5611 Dyna-4, MF 5611 Dyna-6, MF 5612 Dyna-4, MF 5612 Dyna-6, MF 5613 Dyna-4, MF 5613 Dyna-6, MF 6614 Dyna-VT, MF 6614 Dyna-6, MF 6615 Dyna-4, MF 6615 Dyna-VT, MF 6615 Dyna-6, MF 6616 Dyna-VT, MF 6616 Dyna-6, MF 7614 Dyna-4, MF 7615 Dyna-VT, MF 7615 Dyna-6, MF 7615 Dyna-4, MF 7616 Dyna-VT, MF 7616 Dyna-6, MF 7618 Dyna-VT, MF 7618 Dyna-6, MF 7619 Dyna-VT, MF 7619 Dyna-6, MF 7620 Dyna-VT, MF 7620 Dyna-6, MF 7622 Dyna-VT, MF 7622 Dyna-6, MF 7624 Dyna-VT, MF 7624 Dyna-6, MF 5711 SL Dyna-4, MF 5711 SL Dyna-6, MF 5712 SL Dyna-4, MF 5712 SL Dyna-6, MF 5713 SL Dyna-4, MF 5713 SL Dyna-6, MF 6715 S Dyna-4 T4F, MF 6715 S Dyna-6 T4F, MF 6716 S Dyna-6 T4F, MF 7719 Dyna-6, MF 7720 Dyna-6, MF 7722 Dyna-6, MF 7724 Dyna-6, MF 7726 Dyna-6, MF 7714 S Dyna-4, MF 7714 S Dyna-4 T5, MF 7718 S Dyna-VT T5, MF 8727 S Dyna-VT, MF 8730 S Dyna-VT, MF 8732 S Dyna-VT, MF 8735 S Dyna-VT, MF 8737 S Dyna-VT, MF 5465 Dyna-4, MF 5475 Dyna-4, MF 5460 T3 SISU, MF 5445, MF 5470 T3, MF 5480 T3, MF 5465 T3, MF 5475 T3, MF 5445 T3, MF 5455 T3, MF 5450 T3, MF 2670, MF 2680, MF 4708 ECO4, MF 4708 ECO3, MF 4709 ECO3, MF 4707 2WD Non Cab, MF 4708 2WD Non Cab 3, MF 4709 2WD Non Cab, MF 4710 2WD Non Cab, MF 1529, MF 1532H, MF 8660 Dyna-VT T2, MF 8670, MF 8680, MF 8690, MF 8727, MF 8730, MF 8732, MF 8735, MF 5100, MF 9520, MF 9540 Tier 4 TI, MF 9560 Tier 4 TI, MF 9540 T4F, MF 9560 T4F, MF 9245, MF 9565, MF 9895, MF 9695, MF 9795, MF 3000-8-30 Corn Header, MF 3000-8-36 Corn Header, MF 3000-8-38 Corn Header, MF 3000-12-20 Corn Header, MF 3000-12-22 Corn Header, MF 3000-12-30 Corn Header, MF 4200S-13 Pick Up Header, MF 9146, MF 9125, MF 9226, MF 9190, MF 9192, MF 1363, MF WR 9950, MF WR 9960, MF WR 9970, MF WR 9980</t>
+        </is>
+      </c>
+      <c r="D44" s="11" t="inlineStr"/>
     </row>
     <row r="45" ht="18.75" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
@@ -1138,17 +1234,25 @@
           <t>339666X1</t>
         </is>
       </c>
-      <c r="B45" s="11" t="n"/>
-      <c r="C45" s="11" t="n"/>
-      <c r="D45" s="11" t="n"/>
+      <c r="B45" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson, Valtra</t>
+        </is>
+      </c>
+      <c r="C45" s="11" t="inlineStr">
+        <is>
+          <t>PLNTR MOMENTUM 16-30 FT 40', PLNTR MOMENTUM 16-70 FT 40', PLNTR MOMENTUM 16-76 FT 40', PLNTR MOMENTUM 24-20 FT 40', PLNTR MOMENTUM 24-22 FT 40', PLNTR MOMENTUM 32-15 FT 40', PLNTR MOMENTUM 24-30 FT 60', PLNTR MOMENTUM 24-70 FT 60', PLNTR MOMENTUM 24-76 FT 60', PLNTR MOMENTUM 36-20 FT 60', PLNTR MOMENTUM 36-22 FT 60', PLNTR MOMENTUM 48-15 FT 60', 5180E, 8370P, 8400P, 8380P, 8410P, 9300R, 9390R, Cutting table PF 12,2m (40'), Cutting table PF 5,5m (18'), Cutting table PF 7,7m (25'), Cutting table PF 9,2m (30'), Cutting table PF 10,7m (35'), Cutting table FF 7,0m, 9470X, 9490X, 1270 (Serial No. JHBxxx001 to JBHxxx999), 1290 XD (Serial No. JHBxxx001 to JBHxxx999), 12130 (Serial No. JHBxxx001 to JBHxxx999), Squadra 1290 UD, Cutter Middle Attachment, Former 3PT Linkage, Former Lateral Transporter, Former Central Transporter, Former 4r central windr./trans, Former Lateral Swath trailed, Slicer Front Mounted Oscillation, Slicer 3Pt linkage middle attachment, Slicer Mower combinations middle attachment, Slicer trailed, Twister with Transport Chassis, MF 135, MF 165, MF 175, MF 154S 2WD, MF 154S 4WD, MF 174S 2WD, MF 185 4WD, MF 184S 2WD, MF 185S 4WD, MF 174S, MF 154F, MF 174F, MF 184F, MF 194F, MF 194S, MF 154V 2WD, MF 164V, MF 174V 2WD, MF 254S 4WD, MF 294 4WD, MF 264, MF 264 4WD, MF 264S 2WD, MF 264S 4WD, MF 575 4WD, MF 590 4WD, MF 595, MF 595 4WD, MF 592, MF 592 4WD, MF 698, MF 698 4WD, MF 698T, MF 698T 4WD, MF 699, MF 699 4WD, MF 670 4WD, MF 690, MF 3425, MF 3435, MF 3445, MF 3455, MF 354F 2WD, MF 354F 4WD, MF 364F 2WD, MF 364F 4WD, MF 374F 2WD, MF 374F 4WD, MF 384F 2WD, MF 384F 4WD, MF 394F 2WD, MF 394F 4WD, MF 354S 2WD, MF 354S 4WD, MF 364S 2WD, MF 364S 4WD, MF 374S 2WD, MF 374S 4WD, MF 384S 2WD, MF 384S 4WD, MF 394S 2WD, MF 394S 4WD, MF 354V 2WD, MF 354V 4WD, MF 364V 2WD, MF 364V 4WD, MF 374V 2WD, MF 374V 4WD, MF 3435C, MF 3445C, MF 3455C, MF 3425C, MF 3050 2WD, MF 3050 4WD, MF 3060 2WD, MF 3060 4WD, MF 3070 2WD, MF 3070 4WD, MF 3080 2WD, MF 3080 4WD, MF 3090 2WD, MF 3090 4WD, MF 3095 2WD, MF 3095 4WD, MF 3115 2WD, MF 3115 4WD, MF 3125 2WD, MF 3125 4WD, MF 3065 2WD, MF 3065 4WD, MF 3085 2WD, MF 3085 4WD, MF 3120 2WD, MF 3120 4WD, MF 3075 2WD, MF 3075 4WD, MF 3610 2WD, MF 3610 4WD, MF 3630 2WD, MF 3630 4WD, MF 3650 2WD, MF 3650 4WD, MF 3680 2WD, MF 3680 4WD, MF 3645 2WD, MF 3645 4WD, MF 3655 2WD, MF 3655 4WD, MF 3670 2WD, MF 3670 4WD, MF 3690 2WD, MF 3690 4WD, MF 3635 2WD, MF 3635 4WD, MF 294 2WD, MF 284S 2WD, MF 284S 4WD, MF 263, MF 263 4WD, MF 333 2WD, MF 353 2WD, MF 353 4WD, MF 363 2WD, MF 363 4WD, MF 373 2WD, MF 373 4WD, MF 383 2WD, MF 383 4WD, MF 393 2WD, MF 393 4WD, MF 353S 2WD, MF 353S 4WD, MF 363S 4WD, MF 373S 2WD, MF 373S 4WD, MF 377 2WD, MF 377 4WD, MF 387 2WD, MF 387 4WD, MF 397 2WD, MF 397 4WD, MF 364C, MF 1114 4WD, MF 1134 4WD, MF 1014 2WD, MF 1014 4WD, MF 6110 2WD, MF 6110 4WD, MF 6120 2WD, MF 6120 4WD, MF 6130 2WD, MF 6130 4WD, MF 6140 2WD, MF 6140 4WD, MF 6150 2WD, MF 6150 4WD, MF 6160 2WD, MF 6160 4WD, MF 6170 2WD, MF 6170 4WD, MF 6180 2WD, MF 6180 4WD, MF 6190 2WD, MF 6190 4WD, MF 8170 4WD, MF 8110 2WD, MF 8110 4WD, MF 8120 2WD, MF 8120 4WD, MF 8130 2WD, MF 8130 4WD, MF 8140 2WD, MF 8140 4WD, MF 8150 2WD, MF 8150 4WD, MF 8160 2WD, MF 8160 4WD, MF 4315 2WD, MF 4315 4WD, MF 4325 2WD, MF 4325 4WD, MF 4335 2WD, MF 4335 4WD, MF 4345 2WD, MF 4345 4WD, MF 4355 2WD, MF 4355 4WD, MF 4360 2WD, MF 4360 4WD, MF 4365 2WD, MF 4365 4WD, MF 4370 2WD, MF 4370 4WD, MF 4215 2WD, MF 4215 4WD, MF 4220 2WD, MF 4220 4WD, MF 4225 2WD, MF 4225 4WD, MF 4235 2WD, MF 4235 4WD, MF 4240 2WD, MF 4240 4WD, MF 4245 2WD, MF 4245 4WD, MF 4255 2WD, MF 4255 4WD, MF 4260 2WD, MF 4260 4WD, MF 4265 2WD, MF 4265 4WD, MF 4270 2WD, MF 4270 4WD, MF 6290 2WD, MF 6290 4WD, MF 6280 2WD, MF 6280 4WD, MF 6270 2WD, MF 6270 4WD, MF 6265 2WD, MF 6265 4WD, MF 6260 2WD, MF 6260 4WD, MF 6255 2WD, MF 6255 4WD, MF 6245 2WD, MF 6245 4WD, MF 6235 2WD, MF 6235 4WD, MF 8260 4WD, MF 8250 2WD, MF 8250 4WD, MF 8280 4WD, MF 8270 4WD, MF 8260 2WD, MF 8240 2WD, MF 8240 4WD, MF 8220 2WD, MF 8220 4WD, MF 8210 2WD, MF 8210 4WD, 6465 Dyna-6, 6475 Dyna-6, MF 6480 T3 Agco Power, MF 6497 T2 Agco Power, MF 6499 T2 Agco Power, MF 6465 T2 Perkins, MF 6475 T2 Perkins, MF 6480 T2 Perkins, MF 6490 T2 Agco Power, MF 6495 T2 Agco Power, MF 6485 T2 Agco Power, MF 6445 T2 Agco Power, MF 6455 T2 Perkins, MF 6460 T2 Perkins, MF 6470 T2 Perkins, MF 6497 XTRA, MF 6499 XTRA, 6485, MF 6490 T3 Agco Power, MF 6495 T3 Agco Power, MF 6470 T3 Agco Power, MF 6460 T3 Agco Power, 6465, MF 6475 T3 Agco Power, MF 6480 T3 Perkins, MF 6445 T3 Perkins, MF 6455 T3 Perkins, MF 6497 T3 Agco Power, MF 6499 T3 Agco Power, MF 7465 T3 SISU, MF 7475 T3 SISU, MF 7480 T3 SISU, MF 7465, MF 7475, MF 7480, MF 7485, MF 7490, MF 7495, MF 7485 T3, MF 7490 T3, MF 7495 T3, MF 7497, MF 7499, MF 8450, MF 8460, MF 8470, MF 8480, MF 8450 XTRA, MF 8460 XTRA, MF 8470 XTRA, MF 8480 XTRA, MF 9540, MF 9560, MF 9690, MF 9790, MF 9895, MF 9695, MF 9795, MF 2225, MF 2235, MF 2430, MF 2435, MF 2440, MF 2210, MF 2220, MF 2230, MF 8650 T3 / T2, MF 8660 T3 DYNA VT, MF 8670 T3 / T2 DYNA VT, MF 8680 T3 DYNA VT, MF 8690 T3 / T2 DYNA VT, MF 5709 S Dyna-4, MF 5709 S Dyna-6, MF 5608 Dyna-4, MF 5609 Dyna-4, MF 5610 Dyna-4, MF 5611 Dyna-4, MF 5611 Dyna-6, MF 5612 Dyna-4, MF 5612 Dyna-6, MF 5613 Dyna-4, MF 5613 Dyna-6, MF 6612 Dyna-4, MF 6613 Dyna-6, MF 6613 Dyna-4, MF 6614 Dyna-VT, MF 6614 Dyna-6, MF 6615 Dyna-4, MF 6615 Dyna-VT, MF 6615 Dyna-6, MF 6616 Dyna-VT, MF 6616 Dyna-6, MF 7614 Dyna-4, MF 7615 Dyna-VT, MF 7615 Dyna-6, MF 7615 Dyna-4, MF 7616 Dyna-VT, MF 7616 Dyna-6, MF 7618 Dyna-VT, MF 7618 Dyna-6, MF 7619 Dyna-VT, MF 7619 Dyna-6, MF 7620 Dyna-VT, MF 7620 Dyna-6, MF 7622 Dyna-VT, MF 7622 Dyna-6, MF 7624 Dyna-VT, MF 7624 Dyna-6, MF 7626 Dyna-6, MF 5709 SL Dyna-4, MF 5710 SL Dyna-4, MF 5710 SL Dyna-6, MF 5711 SL Dyna-4, MF 5711 SL Dyna-6, MF 5712 SL Dyna-4, MF 5712 SL Dyna-6, MF 5713 SL Dyna-4, MF 5713 SL Dyna-6, MF 6712 S Dyna-4, MF 6713 S Dyna-4, MF 6714 S Dyna-4 T4F, MF 6715 S Dyna-4 T4F, MF 6713 S Dyna-6, MF 6713 S Dyna-VT, MF 6714 S Dyna-6, MF 6714 S Dyna-VT, MF 6715 S Dyna-6 T4F, MF 6715 S Dyna-VT, MF 6716 S Dyna-6 T4F, MF 6716 S Dyna-VT T4F, MF 6718 S Dyna-6, MF 6718 S Dyna-VT, MF 6714 S Dyna-6 T4F, MF 6714 S Dyna-VT T4F, MF 7719 Dyna-6, MF 7715 DYNA-4, MF 7716 Dyna-6, MF 7714 Dyna-4, MF 7715 Dyna-4, MF 7726 Dyna-VT, MF6713 S Dyna-6 T5, MF 6713 S Dyna-VT T5, MF 6714 S Dyna-6 T5, MF 6714 S Dyna-VT T5, MF 6715 S Dyna-6 T5, MF 6715 S Dyna-VT T5, MF 6716 S Dyna-6 T5, MF 6716 S Dyna-VT T5, MF 6718 S Dyna-6 T5, MF 6718 S Dyna-VT T5, MF 7714 S Dyna-4, MF 7719 S Dyna-VT T5, MF 7714 S Dyna-4 T5, MF 7715 S Dyna-VT T5, MF 7715 S Dyna-6 T5, MF 7716 S Dyna-VT T5, MF 7716 S Dyna-6 T5, MF 7718 S Dyna-VT T5, MF 7718 S Dyna-6 T5, MF 8737 S, MF 8727 S Dyna-VT, MF 8730 S Dyna-VT, MF 8732 S Dyna-VT, MF 8735 S Dyna-VT, MF 8737 S Dyna-VT, MF 8740 S Dyna-VT, MF 5465 Dyna-4, MF 5475 Dyna-4, MF 5460 T3 SISU, MF 5445, MF 5455, 5460, 5465, 5475, 5470, MF 5425, MF 5435, MF 5470 T3, MF 5480 T3, MF 5465 T3, MF 5475 T3, MF 5460 SISU, MF 5470 SISU, MF 5445 T3, MF 5455 T3, MF 5410 T3, MF 5420 T3, MF 5430 T3, MF 5440 T3, MF 5450 T3, MF 2170XD, MF 2150 CE, MF 2160 CE, MF 2170CE, MF 185 SII, MF 2140 CE, MF RK 451 TR, MF TD 404-576 Alpine, MF TD 1008-1310 TRC, MF TD 1008-1310 TR-Hyd, MF 265, MF 230, MF8727, MF8730, MF8732, MF8735, MF 8737 MR, MF 350 2WD, MF 350 4WD, MF 375 2WD, MF 375 4WD, MF 390 2WD, MF 390 4WD, MF 398 2WD, MF 398 4WD, MF 399 2WD, MF 399 4WD, MF 360 2WD, MF 360 4WD, MF 365 2WD, MF 365 4WD, MF 355 2WD, MF 355 4WD, MF 390T 2WD, MF 390T 4WD, MF 362 2WD, MF 362 4WD, MF 340 4WD, MF 340 2WD, MF 372 N 2WD, MF 372 N 4WD, MF 382 N 4WD, MF 362 N 2WD, MF 362 N 4WD, MF 342 2WD, MF 352 2WD, MF 7345 S MCS (2011-2014), MF 7347 S MCS (2012-2014), MF 7360 T4I (2012), MF 7360 PL T4I (2012), MF 7370 T4I (2012), MF 7345 S (2011-2014), MF 7347 S (2012-2014), MF 7360 T4I (2013-2014), MF 7360 PL T4I (2013-2014), MF 7370 T4I (2013-2014), MF 7360 PLI T4I (2013-2014), MF 7345 S (09/14 - 08/17), MF 7345 S MCS (09/14 - 08/17), MF 7347 S (09/14 - 08/17), MF 7347 S MCS (09/14 - 08/17), MF 7360 T4F (2015-2017), MF 7360 PL T4F (2015-2017), MF 7360 PLI T4F (2015-2017), MF 7370 T4F (2015-2017), MF 7370 PL (09/14 - 08/17), MF 7340 T4F (2018-2021), MF 7344 TF4 (2018-2021), MF 7345 S T4F (2018-2021), MF 7347 S T4F (2018-2021), MF 7360 T4F (2018-2021), MF 7360 PL/PLI T4F (2018-2021), MF 7370 T4F (2018-2021), MF 7340 ST5 (2021-9999), MF 7344 ST5 (2021-9999), MF 7347 S ST5 (2021-9999), MF 7370 ST5 (2021-9999), MF 7344 (09/15 - 08/17), MF 7382 (04/15 - 03/17), MF 7340 (09/15 - 08/17), MF 7274, MF 7240 (2008-2018), MF 7380 (04/17 - 07/18), MF 7382 (04/17 - 07/18), MF 7370 PLI (2017), MF 7280 (09/08 - 03/13), MF 7282 (09/08 - 03/13), MF 7278, MF 7256, MF 7272, MF Activa S 7345 MCS, MF Activa S 7347 MCS, MF Beta 7360, MF Beta 7370 PL, MF7380, MF7380AL, MF7382, MF9380, MF Beta 7370 PLI, S232 T3, S262 T3, S292 T3 / T2, S322 T3, S352 T3 / T2, No longer used Refer to 11652, No longer used Refer to 11647, No longer used Refer to 11648, No longer used Refer to 11649, No longer used Refer to 11650, No longer used Refer to 11651, T195 (replaced by J3591), T210 (replaced by J3592), T230 (replaced by J3593), T250 (replaced by J3594), A74SH 1C7, A84SH 1C7, A94SH 1C7, A104MH 1C7, A114MH 1C7, A124LH 1C7, A134LH 1C7, A104MH4, A114MH4, N101, S233, S263, S293, S323, S353, S294, S374, S324 SmartTouch MR19, S394 SmartTouch MR19</t>
+        </is>
+      </c>
+      <c r="D45" s="11" t="inlineStr"/>
     </row>
     <row r="46" ht="18.75" customHeight="1">
       <c r="A46" s="4" t="n">
         <v>71399779</v>
       </c>
-      <c r="B46" s="11" t="n"/>
-      <c r="C46" s="11" t="n"/>
-      <c r="D46" s="11" t="n"/>
+      <c r="B46" s="11" t="inlineStr"/>
+      <c r="C46" s="11" t="inlineStr"/>
+      <c r="D46" s="11" t="inlineStr"/>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" s="3" t="inlineStr">
@@ -1156,9 +1260,21 @@
           <t>354671X1</t>
         </is>
       </c>
-      <c r="B47" s="11" t="n"/>
-      <c r="C47" s="11" t="n"/>
-      <c r="D47" s="11" t="n"/>
+      <c r="B47" s="11" t="inlineStr">
+        <is>
+          <t>Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C47" s="11" t="inlineStr">
+        <is>
+          <t>MF 575 4WD, MF 590 4WD, MF 2620/2625, MF 2640/2645 2WD, MF 2640/2645 4WD, MF 2620/2625 4WD, MF 2680 2WD, MF 2680 4WD, MF 2720/2725, MF 3680 4WD, MF 3670 2WD, MF 3670 4WD, MF 3690 2WD, MF 3690 4WD, MF 8150 2WD, MF 8150 4WD, MF 8160 2WD, MF 8160 4WD, MF 9690, MF 9790, MF 375 4WD</t>
+        </is>
+      </c>
+      <c r="D47" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="48" ht="18.75" customHeight="1">
       <c r="A48" s="3" t="inlineStr">
@@ -1166,9 +1282,17 @@
           <t>365775X1</t>
         </is>
       </c>
-      <c r="B48" s="11" t="n"/>
-      <c r="C48" s="11" t="n"/>
-      <c r="D48" s="11" t="n"/>
+      <c r="B48" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C48" s="11" t="inlineStr">
+        <is>
+          <t>9300R, 9390R, MF 155, MF 550, MF 575, MF 560, MF 575 4WD, MF 590 4WD, MF 595, MF 595 4WD, MF 565, MF 592, MF 592 4WD, MF 698, MF 698 4WD, MF 698T, MF 698T 4WD, MF 699, MF 699 4WD, MF 2620/2625, MF 2640/2645 2WD, MF 2640/2645 4WD, MF 2620/2625 4WD, MF 2680 2WD, MF 2680 4WD, MF 2720/2725, MF 1200, MF 8280 4WD, MF 8270 4WD, MF 8260 2WD, MF 9690, MF 9790, MF 9895, MF 9695, MF 9795, MF 298 2WD, MF 298 4WD, MF 290 2WD, MF 290 4WD</t>
+        </is>
+      </c>
+      <c r="D48" s="11" t="inlineStr"/>
     </row>
     <row r="49" ht="18.75" customHeight="1">
       <c r="A49" s="3" t="inlineStr">
@@ -1176,9 +1300,17 @@
           <t>369250X1</t>
         </is>
       </c>
-      <c r="B49" s="11" t="n"/>
-      <c r="C49" s="11" t="n"/>
-      <c r="D49" s="11" t="n"/>
+      <c r="B49" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C49" s="11" t="inlineStr">
+        <is>
+          <t>9300R, 990 (Serial No. JHBxxx001 to JBHxxx999), 1270 (Serial No. JHBxxx001 to JBHxxx999), 1290 XD (Serial No. JHBxxx001 to JBHxxx999), 12130 (Serial No. JHBxxx001 to JBHxxx999), MF 9690, MF 9790, MF 9895, MF 9695, MF 9795, MF 2150 CE, MF 2160 CE, MF 2170CE, MF 185 SII, MF 190CE, MF 186CE, MF 187CE, MF 2140 CE</t>
+        </is>
+      </c>
+      <c r="D49" s="11" t="inlineStr"/>
     </row>
     <row r="50" ht="18.75" customHeight="1">
       <c r="A50" s="3" t="inlineStr">
@@ -1186,9 +1318,17 @@
           <t>WR55261</t>
         </is>
       </c>
-      <c r="B50" s="11" t="n"/>
-      <c r="C50" s="11" t="n"/>
-      <c r="D50" s="11" t="n"/>
+      <c r="B50" s="11" t="inlineStr"/>
+      <c r="C50" s="11" t="inlineStr">
+        <is>
+          <t>7460/7660</t>
+        </is>
+      </c>
+      <c r="D50" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="51" ht="18.75" customHeight="1">
       <c r="A51" s="3" t="inlineStr">
@@ -1196,9 +1336,17 @@
           <t>AG551392</t>
         </is>
       </c>
-      <c r="B51" s="11" t="n"/>
-      <c r="C51" s="11" t="n"/>
-      <c r="D51" s="11" t="n"/>
+      <c r="B51" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C51" s="11" t="inlineStr">
+        <is>
+          <t>PLNTR MOMENTUM 16-30 FT 40', PLNTR MOMENTUM 16-70 FT 40', PLNTR MOMENTUM 16-76 FT 40', PLNTR MOMENTUM 24-20 FT 40', PLNTR MOMENTUM 24-22 FT 40', PLNTR MOMENTUM 32-15 FT 40', PLNTR MOMENTUM 24-30 FT 60', PLNTR MOMENTUM 24-70 FT 60', PLNTR MOMENTUM 24-76 FT 60', PLNTR MOMENTUM 36-20 FT 60', PLNTR MOMENTUM 36-22 FT 60', PLNTR MOMENTUM 48-15 FT 60', 8370P, 8400P, 9300R, 9390R, 9470X, 1270 (Serial No. JHBxxx001 to JBHxxx999), 1290 XD (Serial No. JHBxxx001 to JBHxxx999), 12130 (Serial No. JHBxxx001 to JBHxxx999), 1290, MF 698, MF 699, MF 670 4WD, MF 2640/2645 2WD, MF 3630 2WD, MF 3650 2WD, MF 3680 2WD, MF 3645 2WD, MF 3655 2WD, MF 3670 2WD, MF 3690 2WD, MF 6150 2WD, MF 6170 2WD, MF 6180 2WD, MF 8110 2WD, MF 8120 2WD, MF 8140 2WD, MF 8150 2WD, MF 8160 2WD, MF 9540, MF 9560, MF 9690, MF 9790, MF 9895, MF 9695, MF 9795, MF 2170XD, MF 2150 CE, MF 2160 CE, MF 2170CE, MF 2140 CE, MF 1220 2WD STD, MF 7280 (09/08 - 03/13), MF 7282 (09/08 - 03/13)</t>
+        </is>
+      </c>
+      <c r="D51" s="11" t="inlineStr"/>
     </row>
     <row r="52" ht="18.75" customHeight="1">
       <c r="A52" s="3" t="inlineStr">
@@ -1206,9 +1354,17 @@
           <t>WR10193</t>
         </is>
       </c>
-      <c r="B52" s="11" t="n"/>
-      <c r="C52" s="11" t="n"/>
-      <c r="D52" s="11" t="n"/>
+      <c r="B52" s="11" t="inlineStr">
+        <is>
+          <t>Fendt, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C52" s="11" t="inlineStr">
+        <is>
+          <t>9300R, 9390R, MF 2640/2645 4WD, MF 9690, MF 9790, MF 9895, MF 9695, MF 9795</t>
+        </is>
+      </c>
+      <c r="D52" s="11" t="inlineStr"/>
     </row>
     <row r="53" ht="18.75" customHeight="1">
       <c r="A53" s="3" t="inlineStr">
@@ -1216,9 +1372,13 @@
           <t>SN4845</t>
         </is>
       </c>
-      <c r="B53" s="11" t="n"/>
-      <c r="C53" s="11" t="n"/>
-      <c r="D53" s="11" t="n"/>
+      <c r="B53" s="11" t="inlineStr"/>
+      <c r="C53" s="11" t="inlineStr"/>
+      <c r="D53" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="54" ht="18.75" customHeight="1">
       <c r="A54" s="3" t="inlineStr">
@@ -1226,9 +1386,13 @@
           <t>SN4906</t>
         </is>
       </c>
-      <c r="B54" s="11" t="n"/>
-      <c r="C54" s="11" t="n"/>
-      <c r="D54" s="11" t="n"/>
+      <c r="B54" s="11" t="inlineStr"/>
+      <c r="C54" s="11" t="inlineStr"/>
+      <c r="D54" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="55" ht="18.75" customHeight="1">
       <c r="A55" s="3" t="inlineStr">
@@ -1236,9 +1400,9 @@
           <t>SNFK150219</t>
         </is>
       </c>
-      <c r="B55" s="11" t="n"/>
-      <c r="C55" s="11" t="n"/>
-      <c r="D55" s="11" t="n"/>
+      <c r="B55" s="11" t="inlineStr"/>
+      <c r="C55" s="11" t="inlineStr"/>
+      <c r="D55" s="11" t="inlineStr"/>
     </row>
     <row r="56" ht="18.75" customHeight="1">
       <c r="A56" s="3" t="inlineStr">
@@ -1246,9 +1410,9 @@
           <t>SNFK350402</t>
         </is>
       </c>
-      <c r="B56" s="11" t="n"/>
-      <c r="C56" s="11" t="n"/>
-      <c r="D56" s="11" t="n"/>
+      <c r="B56" s="11" t="inlineStr"/>
+      <c r="C56" s="11" t="inlineStr"/>
+      <c r="D56" s="11" t="inlineStr"/>
     </row>
     <row r="57" ht="18.75" customHeight="1">
       <c r="A57" s="3" t="inlineStr">
@@ -1256,9 +1420,9 @@
           <t>SN6924</t>
         </is>
       </c>
-      <c r="B57" s="11" t="n"/>
-      <c r="C57" s="11" t="n"/>
-      <c r="D57" s="11" t="n"/>
+      <c r="B57" s="11" t="inlineStr"/>
+      <c r="C57" s="11" t="inlineStr"/>
+      <c r="D57" s="11" t="inlineStr"/>
     </row>
     <row r="58" ht="18.75" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
@@ -1266,9 +1430,21 @@
           <t>SN1918</t>
         </is>
       </c>
-      <c r="B58" s="11" t="n"/>
-      <c r="C58" s="11" t="n"/>
-      <c r="D58" s="11" t="n"/>
+      <c r="B58" s="11" t="inlineStr">
+        <is>
+          <t>Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C58" s="11" t="inlineStr">
+        <is>
+          <t>MF 9435</t>
+        </is>
+      </c>
+      <c r="D58" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="59" ht="18.75" customHeight="1">
       <c r="A59" s="3" t="inlineStr">
@@ -1276,9 +1452,13 @@
           <t>SN5530</t>
         </is>
       </c>
-      <c r="B59" s="11" t="n"/>
-      <c r="C59" s="11" t="n"/>
-      <c r="D59" s="11" t="n"/>
+      <c r="B59" s="11" t="inlineStr"/>
+      <c r="C59" s="11" t="inlineStr"/>
+      <c r="D59" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="60" ht="18.75" customHeight="1">
       <c r="A60" s="3" t="inlineStr">
@@ -1286,9 +1466,17 @@
           <t>SN1891</t>
         </is>
       </c>
-      <c r="B60" s="11" t="n"/>
-      <c r="C60" s="11" t="n"/>
-      <c r="D60" s="11" t="n"/>
+      <c r="B60" s="11" t="inlineStr">
+        <is>
+          <t>Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C60" s="11" t="inlineStr">
+        <is>
+          <t>MF 190CE</t>
+        </is>
+      </c>
+      <c r="D60" s="11" t="inlineStr"/>
     </row>
     <row r="61" ht="18.75" customHeight="1">
       <c r="A61" s="3" t="inlineStr">
@@ -1296,9 +1484,21 @@
           <t>SN3485</t>
         </is>
       </c>
-      <c r="B61" s="11" t="n"/>
-      <c r="C61" s="11" t="n"/>
-      <c r="D61" s="11" t="n"/>
+      <c r="B61" s="11" t="inlineStr">
+        <is>
+          <t>Gleaner, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C61" s="11" t="inlineStr">
+        <is>
+          <t>S68, S78, S88, S96, S97, S98, MF 9435</t>
+        </is>
+      </c>
+      <c r="D61" s="11" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
     </row>
     <row r="62" ht="18.75" customHeight="1">
       <c r="A62" s="3" t="inlineStr">
@@ -1306,9 +1506,17 @@
           <t>40646PF</t>
         </is>
       </c>
-      <c r="B62" s="11" t="n"/>
-      <c r="C62" s="11" t="n"/>
-      <c r="D62" s="11" t="n"/>
+      <c r="B62" s="11" t="inlineStr">
+        <is>
+          <t>Challenger, Gleaner, Massey Ferguson</t>
+        </is>
+      </c>
+      <c r="C62" s="11" t="inlineStr">
+        <is>
+          <t>RG900, RG1100, RG1300, RG1100B, RG1300B, 7460/7660, MT525D Dyna-VT, MT535D Dyna-VT, MT545D Dyna-VT, LB34BXD, 2270XD, PTD12 Roller, PTD12 Spoke, 9816 VE, 9824 VE, S67 Super , S77 Super, S68, S78, S88, S96, S97, S98, R65, R66, A66, A76, R76, 5100 Draper Header, 700 Grain Header, 4000 Pickup Header, 4200 Pickup Header, 7000 Grain Header, MF 9435, MF 2670, MF 2680, MF 3000, MF 5100, MF 9520, MF 9540 Tier 4 TI, MF 9560 Tier 4 TI, MF 9540 T4F, MF 9560 T4F, MF 9245, MF 9565, MF 9895, MF 9695, MF 9795, MF 9250-910 DynaFlex SRA, MF 4200S-13 Pick Up Header, MF 1841, MF 1843 N/S, MF 2170XD, MF 2290, MF 2150, MF 2170, MF WR 9430, 9816 VE, 9824 VE</t>
+        </is>
+      </c>
+      <c r="D62" s="11" t="inlineStr"/>
     </row>
     <row r="63" ht="18.75" customHeight="1">
       <c r="A63" s="3" t="inlineStr">

</xml_diff>